<commit_message>
explicit 'boolean' type instead of 'select_one yes_no'
</commit_message>
<xml_diff>
--- a/formats/testdata/formulas.xlsx
+++ b/formats/testdata/formulas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>type</t>
   </si>
@@ -34,9 +34,6 @@
     <t>list name</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>begin group</t>
   </si>
   <si>
@@ -46,18 +43,6 @@
     <t>end group</t>
   </si>
   <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>settings</t>
   </si>
   <si>
@@ -118,7 +103,7 @@
     <t>${show_slide}</t>
   </si>
   <si>
-    <t>select_one yes_no</t>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
@@ -440,7 +425,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,119 +447,119 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -584,10 +569,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,28 +592,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added formula/calculation with tests and documentation
</commit_message>
<xml_diff>
--- a/formats/testdata/formulas.xlsx
+++ b/formats/testdata/formulas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robza\Documents\go\xls2ajf\formats\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnucoop\Documents\go\xls2ajf\formats\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>type</t>
   </si>
@@ -104,6 +104,21 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>calc</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>All true:</t>
+  </si>
+  <si>
+    <t>${show_slide} and ${show_group} and ${show_field}</t>
   </si>
 </sst>
 </file>
@@ -422,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,10 +448,10 @@
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,8 +464,11 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -461,7 +479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -472,7 +490,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -483,7 +501,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -494,71 +512,85 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
constraint implemented and documented and tested
</commit_message>
<xml_diff>
--- a/formats/testdata/formulas.xlsx
+++ b/formats/testdata/formulas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>type</t>
   </si>
@@ -119,6 +119,21 @@
   </si>
   <si>
     <t>${show_slide} and ${show_group} and ${show_field}</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Your age:</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>. &lt; 150</t>
   </si>
 </sst>
 </file>
@@ -437,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,10 +463,11 @@
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,10 +481,13 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -479,7 +498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -490,7 +509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -501,7 +520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -512,7 +531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -522,75 +541,89 @@
       <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
integers added, but still need to figure out the constraint
</commit_message>
<xml_diff>
--- a/formats/testdata/formulas.xlsx
+++ b/formats/testdata/formulas.xlsx
@@ -121,9 +121,6 @@
     <t>${show_slide} and ${show_group} and ${show_field}</t>
   </si>
   <si>
-    <t>decimal</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>age must be less than 150</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,10 +491,10 @@
         <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -557,19 +557,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
table moved in testdata
</commit_message>
<xml_diff>
--- a/formats/testdata/formulas.xlsx
+++ b/formats/testdata/formulas.xlsx
@@ -105,6 +105,45 @@
     <t xml:space="preserve">age must be less than 150</t>
   </si>
   <si>
+    <t xml:space="preserve">end group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${show_slide}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${show_field}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${show_group}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group_field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Field</t>
+  </si>
+  <si>
     <t xml:space="preserve">table</t>
   </si>
   <si>
@@ -112,45 +151,6 @@
   </si>
   <si>
     <t xml:space="preserve">Attendees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${show_slide}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${show_field}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${show_group}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group_field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group Field</t>
   </si>
   <si>
     <t xml:space="preserve">pets_group</t>
@@ -348,10 +348,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -470,35 +470,38 @@
       <c r="A9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>35</v>
@@ -512,7 +515,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>38</v>
@@ -520,29 +523,26 @@
       <c r="C14" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,9 +583,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -728,10 +729,10 @@
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.62"/>
   </cols>
   <sheetData>

</xml_diff>